<commit_message>
added FE services to final architecture
</commit_message>
<xml_diff>
--- a/combined-tasks/fe-services_components_view-models.xlsx
+++ b/combined-tasks/fe-services_components_view-models.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59d27b9184aa6ed4/ulisboa/2-semester/web-applications/aw-project/combined-tasks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E003C7-0D7B-464F-BB77-2D5A83D55364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{09E003C7-0D7B-464F-BB77-2D5A83D55364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43D1934D-6440-E04B-A626-BEECD2EEB5F2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{514BF500-544F-4F68-A0DA-031A64F3E0EF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25160" windowHeight="16680" activeTab="1" xr2:uid="{514BF500-544F-4F68-A0DA-031A64F3E0EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Micro-Frontends (Task1)</t>
   </si>
@@ -184,6 +185,9 @@
   </si>
   <si>
     <t>propsFigure,propsTitle</t>
+  </si>
+  <si>
+    <t>FE Services</t>
   </si>
 </sst>
 </file>
@@ -231,15 +235,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -312,11 +322,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -334,7 +383,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -343,26 +401,44 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,14 +923,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -892,7 +964,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -998,7 +1070,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1140,7 +1212,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1150,21 +1222,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ECBFF23-58CE-4F50-9B61-E6E6390E504D}">
   <dimension ref="C1:G152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63:E69"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.90625" customWidth="1"/>
-    <col min="5" max="5" width="62.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="74.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="62.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="74.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1181,1170 +1253,1175 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C3" s="8" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="16" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C4" s="9"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="12"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C5" s="9"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="9"/>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" s="12"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C6" s="9"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="9"/>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="12"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C7" s="9"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="9"/>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="12"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C8" s="9"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="9"/>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="12"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C9" s="9"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="9"/>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="12"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C10" s="9"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="9"/>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="12"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C11" s="9"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="9"/>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C11" s="12"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C12" s="9"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="9"/>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C12" s="12"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C13" s="9"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="9"/>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C13" s="12"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C14" s="9"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="9"/>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C14" s="12"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C15" s="9"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="9"/>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C15" s="12"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C16" s="9"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="9"/>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C16" s="12"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="12"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="9"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="9"/>
+    <row r="17" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="12"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="9"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="9"/>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C18" s="12"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C19" s="9"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="9"/>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C19" s="12"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="12"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C20" s="9"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="9"/>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C20" s="12"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="12"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C21" s="9"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="9"/>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C21" s="12"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="12"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C22" s="9"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="9"/>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C22" s="12"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="12"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C23" s="9"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="9"/>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C23" s="12"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="12"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C24" s="9"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="9"/>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C24" s="12"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="12"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="3:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="9"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="9"/>
+    <row r="25" spans="3:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="12"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="12"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C26" s="9"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="9"/>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C26" s="12"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="12"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C27" s="9"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="9"/>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C27" s="12"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C28" s="9"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="9"/>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C28" s="12"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="12"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C29" s="9"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="9"/>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C29" s="12"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="12"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C30" s="9"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="9"/>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C30" s="12"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="12"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C31" s="9"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="9"/>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C31" s="12"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="12"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C32" s="10"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="10"/>
+    <row r="32" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="13"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="13"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C33" s="8" t="s">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C33" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="8" t="s">
+      <c r="D33" s="8"/>
+      <c r="E33" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="14" t="s">
         <v>27</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C34" s="9"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C35" s="9"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="9" t="s">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C34" s="12"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C35" s="12"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C36" s="9"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C37" s="9"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="9" t="s">
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C36" s="12"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C37" s="12"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C38" s="9"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C39" s="9"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="9" t="s">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C38" s="12"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C39" s="12"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C40" s="9"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C41" s="9"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="9" t="s">
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C40" s="12"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C41" s="12"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G41" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C42" s="9"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C43" s="9"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="9" t="s">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C42" s="12"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C43" s="12"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C44" s="9"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C45" s="9"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="9" t="s">
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C44" s="12"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C45" s="12"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F45" s="9" t="s">
+      <c r="F45" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G45" s="9" t="s">
+      <c r="G45" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C46" s="9"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-    </row>
-    <row r="47" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C47" s="9"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C48" s="9"/>
-      <c r="D48" s="12"/>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C46" s="12"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="47" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="12"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C48" s="12"/>
+      <c r="D48" s="8"/>
       <c r="E48" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F48" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G48" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C49" s="9"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C50" s="9"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-    </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C51" s="9"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-    </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C52" s="9"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-    </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C53" s="9"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-    </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C54" s="9"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-    </row>
-    <row r="55" spans="3:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C55" s="9"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-    </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C56" s="9"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-    </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C57" s="9"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-    </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C58" s="9"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-    </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C59" s="9"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-    </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C60" s="9"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-    </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C61" s="9"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-    </row>
-    <row r="62" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C62" s="9"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
-    </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C63" s="9"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="8" t="s">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C49" s="12"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C50" s="12"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C51" s="12"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C52" s="12"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C53" s="12"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C54" s="12"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+    </row>
+    <row r="55" spans="3:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="12"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C56" s="12"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C57" s="12"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C58" s="12"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C59" s="12"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C60" s="12"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C61" s="12"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+    </row>
+    <row r="62" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="12"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C63" s="12"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F63" s="8" t="s">
+      <c r="F63" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G63" s="8" t="s">
+      <c r="G63" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C64" s="9"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-    </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C65" s="9"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-    </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C66" s="9"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-    </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C67" s="9"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-    </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C68" s="9"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C69" s="9"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-    </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C70" s="9"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="16" t="s">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C64" s="12"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C65" s="12"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C66" s="12"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C67" s="12"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C68" s="12"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C69" s="12"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C70" s="12"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="9" t="s">
+      <c r="F70" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G70" s="9"/>
-    </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C71" s="9"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-    </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C72" s="9"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-    </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C73" s="9"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-    </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C74" s="9"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-    </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C75" s="9"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-    </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C76" s="9"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-    </row>
-    <row r="77" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C77" s="10"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
-    </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C78" s="8" t="s">
+      <c r="G70" s="12"/>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C71" s="12"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C72" s="12"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C73" s="12"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C74" s="12"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C75" s="12"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C76" s="12"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+    </row>
+    <row r="77" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="13"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C78" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D78" s="12"/>
-      <c r="E78" s="8" t="s">
+      <c r="D78" s="8"/>
+      <c r="E78" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F78" s="8" t="s">
+      <c r="F78" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G78" s="8" t="s">
+      <c r="G78" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C79" s="9"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-    </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C80" s="9"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-    </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C81" s="9"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="9" t="s">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C79" s="12"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C80" s="12"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C81" s="12"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-    </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C82" s="9"/>
-      <c r="D82" s="13"/>
-      <c r="E82" s="9"/>
-      <c r="F82" s="9" t="s">
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C82" s="12"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G82" s="9" t="s">
+      <c r="G82" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C83" s="9"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
-      <c r="G83" s="9"/>
-    </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C84" s="9"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="9" t="s">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C83" s="12"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C84" s="12"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-    </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C85" s="9"/>
-      <c r="D85" s="13"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="9"/>
-      <c r="G85" s="9"/>
-    </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C86" s="9"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9" t="s">
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C85" s="12"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C86" s="12"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G86" s="9" t="s">
+      <c r="G86" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C87" s="9"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="9" t="s">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C87" s="12"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F87" s="9"/>
-      <c r="G87" s="9"/>
-    </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C88" s="9"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
-      <c r="G88" s="9"/>
-    </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C89" s="9"/>
-      <c r="D89" s="13"/>
-      <c r="E89" s="9"/>
-      <c r="F89" s="9"/>
-      <c r="G89" s="9"/>
-    </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C90" s="9"/>
-      <c r="D90" s="13"/>
-      <c r="E90" s="9" t="s">
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C88" s="12"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C89" s="12"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C90" s="12"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F90" s="9" t="s">
+      <c r="F90" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G90" s="9" t="s">
+      <c r="G90" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C91" s="9"/>
-      <c r="D91" s="13"/>
-      <c r="E91" s="9"/>
-      <c r="F91" s="9"/>
-      <c r="G91" s="9"/>
-    </row>
-    <row r="92" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C92" s="9"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="10"/>
-    </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C93" s="9"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="8" t="s">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C91" s="12"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+    </row>
+    <row r="92" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C92" s="12"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C93" s="12"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F93" s="8" t="s">
+      <c r="F93" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G93" s="8" t="s">
+      <c r="G93" s="14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C94" s="9"/>
-      <c r="D94" s="13"/>
-      <c r="E94" s="9"/>
-      <c r="F94" s="9"/>
-      <c r="G94" s="9"/>
-    </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C95" s="9"/>
-      <c r="D95" s="13"/>
-      <c r="E95" s="9"/>
-      <c r="F95" s="9"/>
-      <c r="G95" s="9"/>
-    </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C96" s="9"/>
-      <c r="D96" s="13"/>
-      <c r="E96" s="9"/>
-      <c r="F96" s="9"/>
-      <c r="G96" s="9"/>
-    </row>
-    <row r="97" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C97" s="9"/>
-      <c r="D97" s="13"/>
-      <c r="E97" s="9"/>
-      <c r="F97" s="9"/>
-      <c r="G97" s="9"/>
-    </row>
-    <row r="98" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C98" s="9"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="9" t="s">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C94" s="12"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+    </row>
+    <row r="95" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C95" s="12"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+    </row>
+    <row r="96" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C96" s="12"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12"/>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C97" s="12"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+    </row>
+    <row r="98" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C98" s="12"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F98" s="9"/>
-      <c r="G98" s="9"/>
-    </row>
-    <row r="99" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C99" s="9"/>
-      <c r="D99" s="13"/>
-      <c r="E99" s="9"/>
-      <c r="F99" s="9"/>
-      <c r="G99" s="9"/>
-    </row>
-    <row r="100" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C100" s="9"/>
-      <c r="D100" s="13"/>
-      <c r="E100" s="9"/>
-      <c r="F100" s="9"/>
-      <c r="G100" s="9"/>
-    </row>
-    <row r="101" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C101" s="9"/>
-      <c r="D101" s="13"/>
-      <c r="E101" s="9"/>
-      <c r="F101" s="9"/>
-      <c r="G101" s="9"/>
-    </row>
-    <row r="102" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C102" s="9"/>
-      <c r="D102" s="13"/>
-      <c r="E102" s="9"/>
-      <c r="F102" s="9"/>
-      <c r="G102" s="9"/>
-    </row>
-    <row r="103" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C103" s="9"/>
-      <c r="D103" s="13"/>
-      <c r="E103" s="9" t="s">
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C99" s="12"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C100" s="12"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+    </row>
+    <row r="101" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C101" s="12"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="12"/>
+    </row>
+    <row r="102" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C102" s="12"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12"/>
+    </row>
+    <row r="103" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C103" s="12"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F103" s="9"/>
-      <c r="G103" s="9"/>
-    </row>
-    <row r="104" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C104" s="9"/>
-      <c r="D104" s="13"/>
-      <c r="E104" s="9"/>
-      <c r="F104" s="9"/>
-      <c r="G104" s="9"/>
-    </row>
-    <row r="105" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C105" s="9"/>
-      <c r="D105" s="13"/>
-      <c r="E105" s="9"/>
-      <c r="F105" s="9"/>
-      <c r="G105" s="9"/>
-    </row>
-    <row r="106" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C106" s="9"/>
-      <c r="D106" s="13"/>
-      <c r="E106" s="9"/>
-      <c r="F106" s="9"/>
-      <c r="G106" s="9"/>
-    </row>
-    <row r="107" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C107" s="10"/>
-      <c r="D107" s="14"/>
-      <c r="E107" s="10"/>
-      <c r="F107" s="10"/>
-      <c r="G107" s="10"/>
-    </row>
-    <row r="108" spans="3:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F103" s="12"/>
+      <c r="G103" s="12"/>
+    </row>
+    <row r="104" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C104" s="12"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="12"/>
+      <c r="G104" s="12"/>
+    </row>
+    <row r="105" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C105" s="12"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="12"/>
+      <c r="F105" s="12"/>
+      <c r="G105" s="12"/>
+    </row>
+    <row r="106" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C106" s="12"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="12"/>
+      <c r="F106" s="12"/>
+      <c r="G106" s="12"/>
+    </row>
+    <row r="107" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C107" s="13"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+    </row>
+    <row r="108" spans="3:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C108" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D108" s="12"/>
+      <c r="D108" s="8"/>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
     </row>
-    <row r="109" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C109" s="16"/>
-      <c r="D109" s="13"/>
+    <row r="109" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C109" s="15"/>
+      <c r="D109" s="9"/>
       <c r="E109" s="5"/>
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C110" s="16"/>
-      <c r="D110" s="13"/>
+    <row r="110" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C110" s="15"/>
+      <c r="D110" s="9"/>
       <c r="E110" s="5"/>
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C111" s="16"/>
-      <c r="D111" s="13"/>
+    <row r="111" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C111" s="15"/>
+      <c r="D111" s="9"/>
       <c r="E111" s="5"/>
       <c r="F111" s="5"/>
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C112" s="16"/>
-      <c r="D112" s="13"/>
+    <row r="112" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C112" s="15"/>
+      <c r="D112" s="9"/>
       <c r="E112" s="5"/>
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
     </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C113" s="16"/>
-      <c r="D113" s="13"/>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C113" s="15"/>
+      <c r="D113" s="9"/>
       <c r="E113" s="5"/>
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
     </row>
-    <row r="114" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C114" s="16"/>
-      <c r="D114" s="13"/>
+    <row r="114" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C114" s="15"/>
+      <c r="D114" s="9"/>
       <c r="E114" s="5"/>
       <c r="F114" s="5"/>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C115" s="16"/>
-      <c r="D115" s="13"/>
+    <row r="115" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C115" s="15"/>
+      <c r="D115" s="9"/>
       <c r="E115" s="5"/>
       <c r="F115" s="5"/>
       <c r="G115" s="5"/>
     </row>
-    <row r="116" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C116" s="16"/>
-      <c r="D116" s="13"/>
+    <row r="116" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C116" s="15"/>
+      <c r="D116" s="9"/>
       <c r="E116" s="5"/>
       <c r="F116" s="5"/>
       <c r="G116" s="5"/>
     </row>
-    <row r="117" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C117" s="16"/>
-      <c r="D117" s="13"/>
+    <row r="117" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C117" s="15"/>
+      <c r="D117" s="9"/>
       <c r="E117" s="5"/>
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
     </row>
-    <row r="118" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C118" s="16"/>
-      <c r="D118" s="13"/>
+    <row r="118" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C118" s="15"/>
+      <c r="D118" s="9"/>
       <c r="E118" s="5"/>
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
     </row>
-    <row r="119" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C119" s="16"/>
-      <c r="D119" s="13"/>
+    <row r="119" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C119" s="15"/>
+      <c r="D119" s="9"/>
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
       <c r="G119" s="5"/>
     </row>
-    <row r="120" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C120" s="16"/>
-      <c r="D120" s="13"/>
+    <row r="120" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C120" s="15"/>
+      <c r="D120" s="9"/>
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
       <c r="G120" s="5"/>
     </row>
-    <row r="121" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C121" s="16"/>
-      <c r="D121" s="13"/>
+    <row r="121" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C121" s="15"/>
+      <c r="D121" s="9"/>
       <c r="E121" s="5"/>
       <c r="F121" s="5"/>
       <c r="G121" s="5"/>
     </row>
-    <row r="122" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C122" s="16"/>
-      <c r="D122" s="14"/>
+    <row r="122" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C122" s="15"/>
+      <c r="D122" s="10"/>
       <c r="E122" s="6"/>
       <c r="F122" s="6"/>
       <c r="G122" s="6"/>
     </row>
-    <row r="123" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C123" s="16"/>
-      <c r="D123" s="12"/>
+    <row r="123" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C123" s="15"/>
+      <c r="D123" s="8"/>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
       <c r="G123" s="4"/>
     </row>
-    <row r="124" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C124" s="16"/>
-      <c r="D124" s="13"/>
+    <row r="124" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C124" s="15"/>
+      <c r="D124" s="9"/>
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
       <c r="G124" s="5"/>
     </row>
-    <row r="125" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C125" s="16"/>
-      <c r="D125" s="13"/>
+    <row r="125" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C125" s="15"/>
+      <c r="D125" s="9"/>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
       <c r="G125" s="5"/>
     </row>
-    <row r="126" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C126" s="16"/>
-      <c r="D126" s="13"/>
+    <row r="126" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C126" s="15"/>
+      <c r="D126" s="9"/>
       <c r="E126" s="5"/>
       <c r="F126" s="5"/>
       <c r="G126" s="5"/>
     </row>
-    <row r="127" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C127" s="16"/>
-      <c r="D127" s="13"/>
+    <row r="127" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C127" s="15"/>
+      <c r="D127" s="9"/>
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
       <c r="G127" s="5"/>
     </row>
-    <row r="128" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C128" s="16"/>
-      <c r="D128" s="13"/>
+    <row r="128" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C128" s="15"/>
+      <c r="D128" s="9"/>
       <c r="E128" s="5"/>
       <c r="F128" s="5"/>
       <c r="G128" s="5"/>
     </row>
-    <row r="129" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C129" s="16"/>
-      <c r="D129" s="13"/>
+    <row r="129" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C129" s="15"/>
+      <c r="D129" s="9"/>
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
       <c r="G129" s="5"/>
     </row>
-    <row r="130" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C130" s="16"/>
-      <c r="D130" s="13"/>
+    <row r="130" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C130" s="15"/>
+      <c r="D130" s="9"/>
       <c r="E130" s="7"/>
       <c r="F130" s="5"/>
       <c r="G130" s="5"/>
     </row>
-    <row r="131" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C131" s="16"/>
-      <c r="D131" s="13"/>
+    <row r="131" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C131" s="15"/>
+      <c r="D131" s="9"/>
       <c r="E131" s="5"/>
       <c r="F131" s="5"/>
       <c r="G131" s="5"/>
     </row>
-    <row r="132" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C132" s="16"/>
-      <c r="D132" s="13"/>
+    <row r="132" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C132" s="15"/>
+      <c r="D132" s="9"/>
       <c r="E132" s="5"/>
       <c r="F132" s="5"/>
       <c r="G132" s="5"/>
     </row>
-    <row r="133" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C133" s="16"/>
-      <c r="D133" s="13"/>
+    <row r="133" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C133" s="15"/>
+      <c r="D133" s="9"/>
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
       <c r="G133" s="5"/>
     </row>
-    <row r="134" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C134" s="16"/>
-      <c r="D134" s="13"/>
+    <row r="134" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C134" s="15"/>
+      <c r="D134" s="9"/>
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
       <c r="G134" s="5"/>
     </row>
-    <row r="135" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C135" s="16"/>
-      <c r="D135" s="13"/>
+    <row r="135" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C135" s="15"/>
+      <c r="D135" s="9"/>
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
       <c r="G135" s="5"/>
     </row>
-    <row r="136" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C136" s="16"/>
-      <c r="D136" s="13"/>
+    <row r="136" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C136" s="15"/>
+      <c r="D136" s="9"/>
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
       <c r="G136" s="5"/>
     </row>
-    <row r="137" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C137" s="17"/>
-      <c r="D137" s="14"/>
+      <c r="D137" s="10"/>
       <c r="E137" s="6"/>
       <c r="F137" s="6"/>
       <c r="G137" s="6"/>
     </row>
-    <row r="138" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C138" s="8" t="s">
+    <row r="138" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C138" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D138" s="12"/>
+      <c r="D138" s="8"/>
       <c r="E138" s="4"/>
       <c r="F138" s="4"/>
       <c r="G138" s="4"/>
     </row>
-    <row r="139" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C139" s="9"/>
-      <c r="D139" s="13"/>
+    <row r="139" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C139" s="12"/>
+      <c r="D139" s="9"/>
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
       <c r="G139" s="5"/>
     </row>
-    <row r="140" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C140" s="9"/>
-      <c r="D140" s="13"/>
+    <row r="140" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C140" s="12"/>
+      <c r="D140" s="9"/>
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
       <c r="G140" s="5"/>
     </row>
-    <row r="141" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C141" s="9"/>
-      <c r="D141" s="13"/>
+    <row r="141" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C141" s="12"/>
+      <c r="D141" s="9"/>
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
       <c r="G141" s="5"/>
     </row>
-    <row r="142" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C142" s="9"/>
-      <c r="D142" s="13"/>
+    <row r="142" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C142" s="12"/>
+      <c r="D142" s="9"/>
       <c r="E142" s="5"/>
       <c r="F142" s="5"/>
       <c r="G142" s="5"/>
     </row>
-    <row r="143" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C143" s="9"/>
-      <c r="D143" s="13"/>
+    <row r="143" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C143" s="12"/>
+      <c r="D143" s="9"/>
       <c r="E143" s="5"/>
       <c r="F143" s="5"/>
       <c r="G143" s="5"/>
     </row>
-    <row r="144" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C144" s="9"/>
-      <c r="D144" s="13"/>
+    <row r="144" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C144" s="12"/>
+      <c r="D144" s="9"/>
       <c r="E144" s="5"/>
       <c r="F144" s="5"/>
       <c r="G144" s="5"/>
     </row>
-    <row r="145" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C145" s="9"/>
-      <c r="D145" s="13"/>
+    <row r="145" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C145" s="12"/>
+      <c r="D145" s="9"/>
       <c r="E145" s="5"/>
       <c r="F145" s="5"/>
       <c r="G145" s="5"/>
     </row>
-    <row r="146" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C146" s="9"/>
-      <c r="D146" s="13"/>
+    <row r="146" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C146" s="12"/>
+      <c r="D146" s="9"/>
       <c r="E146" s="5"/>
       <c r="F146" s="5"/>
       <c r="G146" s="5"/>
     </row>
-    <row r="147" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C147" s="9"/>
-      <c r="D147" s="13"/>
+    <row r="147" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C147" s="12"/>
+      <c r="D147" s="9"/>
       <c r="E147" s="5"/>
       <c r="F147" s="5"/>
       <c r="G147" s="5"/>
     </row>
-    <row r="148" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C148" s="9"/>
-      <c r="D148" s="13"/>
+    <row r="148" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C148" s="12"/>
+      <c r="D148" s="9"/>
       <c r="E148" s="5"/>
       <c r="F148" s="5"/>
       <c r="G148" s="5"/>
     </row>
-    <row r="149" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C149" s="9"/>
-      <c r="D149" s="13"/>
+    <row r="149" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C149" s="12"/>
+      <c r="D149" s="9"/>
       <c r="E149" s="5"/>
       <c r="F149" s="5"/>
       <c r="G149" s="5"/>
     </row>
-    <row r="150" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C150" s="9"/>
-      <c r="D150" s="13"/>
+    <row r="150" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C150" s="12"/>
+      <c r="D150" s="9"/>
       <c r="E150" s="5"/>
       <c r="F150" s="5"/>
       <c r="G150" s="5"/>
     </row>
-    <row r="151" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C151" s="9"/>
-      <c r="D151" s="13"/>
+    <row r="151" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C151" s="12"/>
+      <c r="D151" s="9"/>
       <c r="E151" s="5"/>
       <c r="F151" s="5"/>
       <c r="G151" s="5"/>
     </row>
-    <row r="152" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C152" s="10"/>
-      <c r="D152" s="14"/>
+    <row r="152" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C152" s="13"/>
+      <c r="D152" s="10"/>
       <c r="E152" s="6"/>
       <c r="F152" s="6"/>
       <c r="G152" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="D48:D62"/>
-    <mergeCell ref="D63:D77"/>
-    <mergeCell ref="D3:D17"/>
-    <mergeCell ref="D18:D32"/>
-    <mergeCell ref="D33:D47"/>
-    <mergeCell ref="E48:E62"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="E93:E97"/>
-    <mergeCell ref="E98:E102"/>
-    <mergeCell ref="E103:E107"/>
-    <mergeCell ref="E63:E69"/>
-    <mergeCell ref="E70:E77"/>
+    <mergeCell ref="F93:F107"/>
+    <mergeCell ref="G93:G107"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="F82:F85"/>
+    <mergeCell ref="F86:F89"/>
+    <mergeCell ref="F90:F92"/>
+    <mergeCell ref="G78:G81"/>
+    <mergeCell ref="G82:G85"/>
+    <mergeCell ref="G86:G89"/>
+    <mergeCell ref="G90:G92"/>
+    <mergeCell ref="F63:F69"/>
+    <mergeCell ref="G48:G62"/>
+    <mergeCell ref="F48:F62"/>
+    <mergeCell ref="G63:G77"/>
+    <mergeCell ref="F70:F77"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="F37:F40"/>
+    <mergeCell ref="F41:F44"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="G33:G36"/>
+    <mergeCell ref="G37:G40"/>
+    <mergeCell ref="G41:G44"/>
+    <mergeCell ref="G45:G47"/>
     <mergeCell ref="C138:C152"/>
     <mergeCell ref="D138:D152"/>
     <mergeCell ref="E3:E32"/>
@@ -2361,29 +2438,24 @@
     <mergeCell ref="E84:E86"/>
     <mergeCell ref="E87:E89"/>
     <mergeCell ref="E90:E92"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="F37:F40"/>
-    <mergeCell ref="F41:F44"/>
-    <mergeCell ref="F45:F47"/>
-    <mergeCell ref="G33:G36"/>
-    <mergeCell ref="G37:G40"/>
-    <mergeCell ref="G41:G44"/>
-    <mergeCell ref="G45:G47"/>
-    <mergeCell ref="F63:F69"/>
-    <mergeCell ref="G48:G62"/>
-    <mergeCell ref="F48:F62"/>
-    <mergeCell ref="G63:G77"/>
-    <mergeCell ref="F70:F77"/>
-    <mergeCell ref="F78:F81"/>
-    <mergeCell ref="F82:F85"/>
-    <mergeCell ref="F86:F89"/>
-    <mergeCell ref="F90:F92"/>
-    <mergeCell ref="G78:G81"/>
-    <mergeCell ref="G82:G85"/>
-    <mergeCell ref="G86:G89"/>
-    <mergeCell ref="G90:G92"/>
-    <mergeCell ref="F93:F107"/>
-    <mergeCell ref="G93:G107"/>
+    <mergeCell ref="E93:E97"/>
+    <mergeCell ref="E98:E102"/>
+    <mergeCell ref="E103:E107"/>
+    <mergeCell ref="E63:E69"/>
+    <mergeCell ref="E70:E77"/>
+    <mergeCell ref="E48:E62"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="D48:D62"/>
+    <mergeCell ref="D63:D77"/>
+    <mergeCell ref="D3:D17"/>
+    <mergeCell ref="D18:D32"/>
+    <mergeCell ref="D33:D47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2392,6 +2464,316 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34044D5C-E095-1145-9B28-F7FFACB22223}">
+  <dimension ref="A1:K35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E7" s="20"/>
+      <c r="F7" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="28"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E8" s="20"/>
+      <c r="F8" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E9" s="20"/>
+      <c r="F9" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="27"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E10" s="20"/>
+      <c r="F10" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="26"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E13" s="20"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E14" s="20"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E15" s="20"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E16" s="20"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E17" s="20"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E18" s="20"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E19" s="20"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E21" s="20"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E22" s="20"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+    </row>
+    <row r="26" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+    </row>
+    <row r="27" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+    </row>
+    <row r="28" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+    </row>
+    <row r="29" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+    </row>
+    <row r="30" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+    </row>
+    <row r="31" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+    </row>
+    <row r="32" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+    </row>
+    <row r="33" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+    </row>
+    <row r="34" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+    </row>
+    <row r="35" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85136C7-D4D2-484A-AF49-850F6239AA1C}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2399,7 +2781,7 @@
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>